<commit_message>
* Effect Manager 초안 구현.  * Asset ID 초안 구현.
</commit_message>
<xml_diff>
--- a/input/Domains/Sound/tables/SoundTable.xlsx
+++ b/input/Domains/Sound/tables/SoundTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devian\input\Domains\Sound\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7647EDD-169C-48C8-B899-253E799EFC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99416D33-7191-4866-B61F-9451A3804310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="900" windowWidth="25635" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="900" windowWidth="25635" windowHeight="13905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOUND" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>bgm_title</t>
   </si>
   <si>
-    <t>sound</t>
-  </si>
-  <si>
     <t>BGM_Title</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>hello</t>
   </si>
   <si>
-    <t>greet</t>
-  </si>
-  <si>
     <t>voice_hello_ko</t>
   </si>
   <si>
@@ -174,6 +168,14 @@
   </si>
   <si>
     <t>voice_bye_ja</t>
+  </si>
+  <si>
+    <t>sounds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>voices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -522,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -643,13 +645,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -684,19 +686,19 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -731,19 +733,19 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -778,19 +780,19 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -825,19 +827,19 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -872,19 +874,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>34</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -919,19 +921,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -971,13 +973,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -1004,16 +1009,16 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>40</v>
-      </c>
-      <c r="M1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1064,10 +1069,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1091,21 +1096,21 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
         <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1129,13 +1134,13 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" t="s">
         <v>48</v>
-      </c>
-      <c r="K6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L6" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Table에 Group key 추가 및 Editor ID 선택 창에 선택 하도록 수정.
</commit_message>
<xml_diff>
--- a/input/Domains/Sound/tables/SoundTable.xlsx
+++ b/input/Domains/Sound/tables/SoundTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Devwinsoft\devian\input\Domains\Sound\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99416D33-7191-4866-B61F-9451A3804310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64088142-E93D-4AC2-BC49-965960660A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="900" windowWidth="25635" windowHeight="13905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="900" windowWidth="25635" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOUND" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>row_id</t>
   </si>
@@ -175,6 +175,10 @@
   </si>
   <si>
     <t>voices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group:true</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -627,6 +631,9 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -973,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>